<commit_message>
completed MARACOOS closes #33
</commit_message>
<xml_diff>
--- a/2021/data/processed/MARACOOS.xlsx
+++ b/2021/data/processed/MARACOOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathew.Biddle\Documents\GitProjects\ioos-asset-inventory\2021\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D6D9C9-26F8-4B72-8043-C467685497A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887FA330-418F-4B21-A0FC-08D6DE1214A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23955" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1101,8 +1101,8 @@
   <dimension ref="A1:Z44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1191,33 +1191,95 @@
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
     </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="9">
+        <v>38.781300000000002</v>
+      </c>
+      <c r="G2" s="9">
+        <v>-76.713700000000003</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="8">
+        <v>2003</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="10"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="9">
-        <v>38.781300000000002</v>
+        <v>39.285400000000003</v>
       </c>
       <c r="G3" s="9">
-        <v>-76.713700000000003</v>
+        <v>-76.608800000000002</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="8">
-        <v>2003</v>
+        <v>2016</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>24</v>
@@ -1253,33 +1315,95 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
     </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="9">
+        <v>39.285499999999999</v>
+      </c>
+      <c r="G4" s="9">
+        <v>-76.608000000000004</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2016</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="10"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="9">
-        <v>39.285400000000003</v>
+        <v>39.0075</v>
       </c>
       <c r="G5" s="9">
-        <v>-76.608800000000002</v>
+        <v>-76.400300000000001</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="8">
-        <v>2016</v>
+        <v>2004</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>24</v>
@@ -1320,28 +1444,28 @@
         <v>18</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="9">
-        <v>39.285499999999999</v>
+        <v>39.450800000000001</v>
       </c>
       <c r="G6" s="9">
-        <v>-76.608000000000004</v>
+        <v>-76.274600000000007</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="8">
-        <v>2016</v>
+        <v>2003</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>24</v>
@@ -1377,33 +1501,95 @@
       <c r="Y6" s="11"/>
       <c r="Z6" s="11"/>
     </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="9">
+        <v>39.213500000000003</v>
+      </c>
+      <c r="G7" s="9">
+        <v>-76.246200000000002</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="8">
+        <v>2015</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="10"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="9">
-        <v>39.0075</v>
+        <v>38.208599999999997</v>
       </c>
       <c r="G8" s="9">
-        <v>-76.400300000000001</v>
+        <v>-75.804599999999994</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="8">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>24</v>
@@ -1439,57 +1625,181 @@
       <c r="Y8" s="11"/>
       <c r="Z8" s="11"/>
     </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="9">
+        <v>40.721538000000002</v>
+      </c>
+      <c r="G9" s="9">
+        <v>-74.015600000000006</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="8">
+        <v>2016</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="R9" s="10"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="9">
+        <v>40.764628000000002</v>
+      </c>
+      <c r="G10" s="9">
+        <v>-74.003185999999999</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="8">
+        <v>2012</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="R10" s="10"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>46</v>
+      <c r="B11" s="13" t="s">
+        <v>89</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="F11" s="9">
-        <v>39.450800000000001</v>
+        <v>42.830199999999998</v>
       </c>
       <c r="G11" s="9">
-        <v>-76.274600000000007</v>
+        <v>-73.992500000000007</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="8">
-        <v>2003</v>
+        <v>2012</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>26</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>28</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
       <c r="R11" s="10"/>
       <c r="S11" s="11"/>
@@ -1505,53 +1815,53 @@
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>48</v>
+      <c r="B12" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="F12" s="9">
-        <v>39.213500000000003</v>
+        <v>42.828099999999999</v>
       </c>
       <c r="G12" s="9">
-        <v>-76.246200000000002</v>
+        <v>-73.990399999999994</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="8">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>26</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="P12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="R12" s="10"/>
       <c r="S12" s="11"/>
@@ -1563,57 +1873,181 @@
       <c r="Y12" s="11"/>
       <c r="Z12" s="11"/>
     </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="9">
+        <v>41.386099999999999</v>
+      </c>
+      <c r="G13" s="9">
+        <v>-73.954999999999998</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="8">
+        <v>2016</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="R13" s="10"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="11"/>
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="9">
+        <v>41.831876000000001</v>
+      </c>
+      <c r="G14" s="9">
+        <v>-73.941605999999993</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="8">
+        <v>2008</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="R14" s="10"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>54</v>
+      <c r="B15" s="13" t="s">
+        <v>102</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="F15" s="9">
-        <v>38.208599999999997</v>
+        <v>42.850999999999999</v>
       </c>
       <c r="G15" s="9">
-        <v>-75.804599999999994</v>
+        <v>-73.887</v>
       </c>
       <c r="H15" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="8">
-        <v>2006</v>
+        <v>2014</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>26</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="O15" s="8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="P15" s="8" t="s">
         <v>28</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="R15" s="10"/>
       <c r="S15" s="11"/>
@@ -1625,33 +2059,281 @@
       <c r="Y15" s="11"/>
       <c r="Z15" s="11"/>
     </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="9">
+        <v>42.501199999999997</v>
+      </c>
+      <c r="G16" s="9">
+        <v>-73.780381000000006</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="8">
+        <v>2013</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="R16" s="10"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="11"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+    </row>
+    <row r="17" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="9">
+        <v>42.499600000000001</v>
+      </c>
+      <c r="G17" s="9">
+        <v>-73.776799999999994</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="8">
+        <v>2008</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="R17" s="10"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="11"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+    </row>
+    <row r="18" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="9">
+        <v>42.619540000000001</v>
+      </c>
+      <c r="G18" s="9">
+        <v>-73.758899999999997</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="8">
+        <v>2011</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q18" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="R18" s="10"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+    </row>
+    <row r="19" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="9">
+        <v>41.042999999999999</v>
+      </c>
+      <c r="G19" s="9">
+        <v>-73.896000000000001</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="8">
+        <v>2008</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="R19" s="10"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+    </row>
     <row r="20" spans="1:26" ht="14.25" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F20" s="9">
-        <v>40.721538000000002</v>
+      <c r="F20" s="14">
+        <v>41.720599999999997</v>
       </c>
       <c r="G20" s="9">
-        <v>-74.015600000000006</v>
+        <v>-73.938800000000001</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I20" s="8">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>24</v>
@@ -1675,7 +2357,7 @@
         <v>28</v>
       </c>
       <c r="Q20" s="8" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="R20" s="10"/>
       <c r="S20" s="11"/>
@@ -1691,53 +2373,53 @@
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>87</v>
+      <c r="B21" s="15" t="s">
+        <v>114</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>20</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>83</v>
+        <v>22</v>
       </c>
       <c r="F21" s="9">
-        <v>40.764628000000002</v>
+        <v>39.244700000000002</v>
       </c>
       <c r="G21" s="9">
-        <v>-74.003185999999999</v>
+        <v>-76.597200000000001</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="8">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="J21" s="8" t="s">
         <v>24</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>26</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="N21" s="8" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="O21" s="8" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="P21" s="8" t="s">
         <v>28</v>
       </c>
       <c r="Q21" s="8" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="R21" s="10"/>
       <c r="S21" s="11"/>
@@ -1750,1430 +2432,1452 @@
       <c r="Z21" s="11"/>
     </row>
     <row r="22" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>89</v>
+      <c r="B22" s="17" t="s">
+        <v>116</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F22" s="9">
-        <v>42.830199999999998</v>
-      </c>
-      <c r="G22" s="9">
-        <v>-73.992500000000007</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I22" s="8">
-        <v>2012</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L22" s="8" t="s">
+      <c r="D22" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="18">
+        <v>39.271700000000003</v>
+      </c>
+      <c r="G22" s="18">
+        <v>-73.889200000000002</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="I22" s="19">
+        <v>44013</v>
+      </c>
+      <c r="J22" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="M22" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O22" s="8" t="s">
-        <v>84</v>
+      <c r="K22" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="P22" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q22" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="R22" s="10"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
+      <c r="Q22" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="21"/>
+      <c r="U22" s="21"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="21"/>
+      <c r="Z22" s="21"/>
     </row>
     <row r="23" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>92</v>
+      <c r="B23" s="17" t="s">
+        <v>124</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" s="9">
-        <v>42.828099999999999</v>
-      </c>
-      <c r="G23" s="9">
-        <v>-73.990399999999994</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I23" s="8">
-        <v>2012</v>
-      </c>
-      <c r="J23" s="8" t="s">
+      <c r="D23" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="22">
+        <v>39.202500000000001</v>
+      </c>
+      <c r="G23" s="23">
+        <v>-74.081940000000003</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="I23" s="24">
+        <v>44330</v>
+      </c>
+      <c r="J23" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K23" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L23" s="8" t="s">
+      <c r="K23" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="L23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M23" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N23" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O23" s="8" t="s">
-        <v>84</v>
+      <c r="M23" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="N23" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="P23" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q23" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="R23" s="10"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="11"/>
+      <c r="Q23" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="21"/>
+      <c r="Z23" s="21"/>
     </row>
     <row r="24" spans="1:26" ht="14.25" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F24" s="9">
-        <v>41.386099999999999</v>
-      </c>
-      <c r="G24" s="9">
-        <v>-73.954999999999998</v>
-      </c>
-      <c r="H24" s="8" t="s">
+      <c r="D24" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" s="12">
+        <v>36.904629999999997</v>
+      </c>
+      <c r="G24" s="12">
+        <v>-75.712649999999996</v>
+      </c>
+      <c r="H24" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="8">
-        <v>2016</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L24" s="8" t="s">
+      <c r="I24" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J24" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M24" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="N24" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O24" s="8" t="s">
-        <v>84</v>
+      <c r="K24" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L24" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="N24" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O24" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="P24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q24" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="R24" s="10"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
+      <c r="Q24" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="29"/>
+      <c r="X24" s="29"/>
+      <c r="Y24" s="29"/>
+      <c r="Z24" s="29"/>
     </row>
     <row r="25" spans="1:26" ht="14.25" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>99</v>
+      <c r="B25" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="9">
-        <v>41.831876000000001</v>
-      </c>
-      <c r="G25" s="9">
-        <v>-73.941605999999993</v>
-      </c>
-      <c r="H25" s="8" t="s">
+      <c r="D25" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="12">
+        <v>36.945230000000002</v>
+      </c>
+      <c r="G25" s="12">
+        <v>-76.391450000000006</v>
+      </c>
+      <c r="H25" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="8">
-        <v>2008</v>
-      </c>
-      <c r="J25" s="8" t="s">
+      <c r="I25" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J25" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K25" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L25" s="8" t="s">
+      <c r="K25" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L25" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M25" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O25" s="8" t="s">
-        <v>84</v>
+      <c r="M25" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="N25" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O25" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="P25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q25" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="R25" s="10"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="11"/>
+      <c r="Q25" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
+      <c r="T25" s="29"/>
+      <c r="U25" s="29"/>
+      <c r="V25" s="29"/>
+      <c r="W25" s="29"/>
+      <c r="X25" s="29"/>
+      <c r="Y25" s="29"/>
+      <c r="Z25" s="29"/>
     </row>
     <row r="26" spans="1:26" ht="14.25" customHeight="1">
       <c r="A26" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>102</v>
+      <c r="B26" s="28" t="s">
+        <v>135</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="9">
-        <v>42.850999999999999</v>
-      </c>
-      <c r="G26" s="9">
-        <v>-73.887</v>
-      </c>
-      <c r="H26" s="8" t="s">
+      <c r="D26" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F26" s="12">
+        <v>37.787990000000001</v>
+      </c>
+      <c r="G26" s="12">
+        <v>-75.973500000000001</v>
+      </c>
+      <c r="H26" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="8">
-        <v>2014</v>
-      </c>
-      <c r="J26" s="8" t="s">
+      <c r="I26" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J26" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K26" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L26" s="8" t="s">
+      <c r="K26" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L26" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M26" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N26" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O26" s="8" t="s">
-        <v>84</v>
+      <c r="M26" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="N26" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O26" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="P26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q26" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="R26" s="10"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
-      <c r="Z26" s="11"/>
+      <c r="Q26" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
+      <c r="V26" s="29"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
+      <c r="Y26" s="29"/>
+      <c r="Z26" s="29"/>
     </row>
     <row r="27" spans="1:26" ht="14.25" customHeight="1">
       <c r="A27" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>104</v>
+      <c r="B27" s="28" t="s">
+        <v>137</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="9">
-        <v>42.501199999999997</v>
-      </c>
-      <c r="G27" s="9">
-        <v>-73.780381000000006</v>
-      </c>
-      <c r="H27" s="8" t="s">
+      <c r="D27" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" s="12">
+        <v>36.9178</v>
+      </c>
+      <c r="G27" s="12">
+        <v>-76.090450000000004</v>
+      </c>
+      <c r="H27" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="8">
-        <v>2013</v>
-      </c>
-      <c r="J27" s="8" t="s">
+      <c r="I27" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J27" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K27" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L27" s="8" t="s">
+      <c r="K27" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L27" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M27" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N27" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O27" s="8" t="s">
-        <v>84</v>
+      <c r="M27" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O27" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="P27" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q27" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="R27" s="10"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
+      <c r="Q27" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="29"/>
+      <c r="U27" s="29"/>
+      <c r="V27" s="29"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="29"/>
     </row>
     <row r="28" spans="1:26" ht="14.25" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>106</v>
+      <c r="B28" s="28" t="s">
+        <v>139</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" s="9">
-        <v>42.499600000000001</v>
-      </c>
-      <c r="G28" s="9">
-        <v>-73.776799999999994</v>
-      </c>
-      <c r="H28" s="8" t="s">
+      <c r="D28" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F28" s="12">
+        <v>38.326990000000002</v>
+      </c>
+      <c r="G28" s="12">
+        <v>-75.083209999999994</v>
+      </c>
+      <c r="H28" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I28" s="8">
-        <v>2008</v>
-      </c>
-      <c r="J28" s="8" t="s">
+      <c r="I28" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J28" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K28" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L28" s="8" t="s">
+      <c r="K28" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L28" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M28" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N28" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O28" s="8" t="s">
-        <v>84</v>
+      <c r="M28" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="N28" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O28" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="P28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q28" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="R28" s="10"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
+      <c r="Q28" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+      <c r="T28" s="29"/>
+      <c r="U28" s="29"/>
+      <c r="V28" s="29"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="29"/>
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29"/>
     </row>
     <row r="29" spans="1:26" ht="14.25" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>108</v>
+      <c r="B29" s="28" t="s">
+        <v>141</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" s="9">
-        <v>42.619540000000001</v>
-      </c>
-      <c r="G29" s="9">
-        <v>-73.758899999999997</v>
-      </c>
-      <c r="H29" s="8" t="s">
+      <c r="D29" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="12">
+        <v>36.927059999999997</v>
+      </c>
+      <c r="G29" s="12">
+        <v>-76.006649999999993</v>
+      </c>
+      <c r="H29" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I29" s="8">
-        <v>2011</v>
-      </c>
-      <c r="J29" s="8" t="s">
+      <c r="I29" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J29" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="K29" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L29" s="8" t="s">
+      <c r="K29" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L29" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M29" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N29" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O29" s="8" t="s">
-        <v>84</v>
+      <c r="M29" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="N29" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O29" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="P29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q29" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="R29" s="10"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-      <c r="U29" s="11"/>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="11"/>
-      <c r="Z29" s="11"/>
+      <c r="Q29" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
+      <c r="T29" s="29"/>
+      <c r="U29" s="29"/>
+      <c r="V29" s="29"/>
+      <c r="W29" s="29"/>
+      <c r="X29" s="29"/>
+      <c r="Y29" s="29"/>
+      <c r="Z29" s="29"/>
     </row>
     <row r="30" spans="1:26" ht="14.25" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>110</v>
+      <c r="B30" s="28" t="s">
+        <v>143</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" s="9">
-        <v>41.042999999999999</v>
-      </c>
-      <c r="G30" s="9">
-        <v>-73.896000000000001</v>
-      </c>
-      <c r="H30" s="8" t="s">
+      <c r="D30" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="12">
+        <v>37.601660000000003</v>
+      </c>
+      <c r="G30" s="12">
+        <v>-75.68974</v>
+      </c>
+      <c r="H30" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I30" s="8">
-        <v>2008</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L30" s="8" t="s">
+      <c r="I30" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J30" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M30" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N30" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O30" s="8" t="s">
-        <v>84</v>
+      <c r="K30" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L30" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M30" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="N30" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O30" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="P30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q30" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="R30" s="10"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="11"/>
+      <c r="Q30" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+      <c r="T30" s="29"/>
+      <c r="U30" s="29"/>
+      <c r="V30" s="29"/>
+      <c r="W30" s="29"/>
+      <c r="X30" s="29"/>
+      <c r="Y30" s="29"/>
+      <c r="Z30" s="29"/>
     </row>
     <row r="31" spans="1:26" ht="14.25" customHeight="1">
       <c r="A31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>112</v>
+      <c r="B31" s="28" t="s">
+        <v>145</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="14">
-        <v>41.720599999999997</v>
-      </c>
-      <c r="G31" s="9">
-        <v>-73.938800000000001</v>
-      </c>
-      <c r="H31" s="8" t="s">
+      <c r="D31" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F31" s="12">
+        <v>36.589709999999997</v>
+      </c>
+      <c r="G31" s="12">
+        <v>-76.020989999999998</v>
+      </c>
+      <c r="H31" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="8">
-        <v>2012</v>
-      </c>
-      <c r="J31" s="8" t="s">
+      <c r="I31" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K31" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="L31" s="8" t="s">
+      <c r="K31" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L31" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M31" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="N31" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="O31" s="8" t="s">
-        <v>84</v>
+      <c r="M31" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="N31" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O31" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="P31" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q31" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="R31" s="10"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="11"/>
-      <c r="Z31" s="11"/>
+      <c r="Q31" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="R31" s="29"/>
+      <c r="S31" s="29"/>
+      <c r="T31" s="29"/>
+      <c r="U31" s="29"/>
+      <c r="V31" s="29"/>
+      <c r="W31" s="29"/>
+      <c r="X31" s="29"/>
+      <c r="Y31" s="29"/>
+      <c r="Z31" s="29"/>
     </row>
     <row r="32" spans="1:26" ht="14.25" customHeight="1">
       <c r="A32" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>114</v>
+      <c r="B32" s="28" t="s">
+        <v>147</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="9">
-        <v>39.244700000000002</v>
-      </c>
-      <c r="G32" s="9">
-        <v>-76.597200000000001</v>
-      </c>
-      <c r="H32" s="8" t="s">
+      <c r="D32" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F32" s="12">
+        <v>37.036520000000003</v>
+      </c>
+      <c r="G32" s="12">
+        <v>-76.076660000000004</v>
+      </c>
+      <c r="H32" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="8">
-        <v>2013</v>
-      </c>
-      <c r="J32" s="8" t="s">
+      <c r="I32" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J32" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="K32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L32" s="8" t="s">
+      <c r="K32" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L32" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="M32" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N32" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O32" s="8" t="s">
-        <v>25</v>
+      <c r="M32" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="N32" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="O32" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="P32" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R32" s="10"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
+      <c r="Q32" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="R32" s="29"/>
+      <c r="S32" s="29"/>
+      <c r="T32" s="29"/>
+      <c r="U32" s="29"/>
+      <c r="V32" s="29"/>
+      <c r="W32" s="29"/>
+      <c r="X32" s="29"/>
+      <c r="Y32" s="29"/>
+      <c r="Z32" s="29"/>
     </row>
     <row r="33" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="17" t="s">
-        <v>116</v>
+      <c r="B33" s="28" t="s">
+        <v>149</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="16" t="s">
-        <v>117</v>
+      <c r="D33" s="28" t="s">
+        <v>150</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F33" s="18">
-        <v>39.271700000000003</v>
-      </c>
-      <c r="G33" s="18">
-        <v>-73.889200000000002</v>
+        <v>129</v>
+      </c>
+      <c r="F33" s="12">
+        <v>36.830370000000002</v>
+      </c>
+      <c r="G33" s="12">
+        <v>-75.966570000000004</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="I33" s="19">
-        <v>44013</v>
-      </c>
-      <c r="J33" s="20" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="I33" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="L33" s="16" t="s">
         <v>26</v>
       </c>
       <c r="M33" s="16" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="N33" s="16" t="s">
         <v>122</v>
       </c>
       <c r="O33" s="16" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="P33" s="8" t="s">
         <v>28</v>
       </c>
       <c r="Q33" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="R33" s="21"/>
-      <c r="S33" s="21"/>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
-      <c r="V33" s="21"/>
-      <c r="W33" s="21"/>
-      <c r="X33" s="21"/>
-      <c r="Y33" s="21"/>
-      <c r="Z33" s="21"/>
+        <v>132</v>
+      </c>
+      <c r="R33" s="29"/>
+      <c r="S33" s="29"/>
+      <c r="T33" s="29"/>
+      <c r="U33" s="29"/>
+      <c r="V33" s="29"/>
+      <c r="W33" s="29"/>
+      <c r="X33" s="29"/>
+      <c r="Y33" s="29"/>
+      <c r="Z33" s="29"/>
     </row>
     <row r="34" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="17" t="s">
-        <v>124</v>
+      <c r="B34" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" s="22">
-        <v>39.202500000000001</v>
-      </c>
-      <c r="G34" s="23">
-        <v>-74.081940000000003</v>
-      </c>
-      <c r="H34" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="I34" s="24">
-        <v>44330</v>
-      </c>
-      <c r="J34" s="16" t="s">
+      <c r="D34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" s="9">
+        <v>38.795999999999999</v>
+      </c>
+      <c r="G34" s="9">
+        <v>-76.720799999999997</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="8">
+        <v>2003</v>
+      </c>
+      <c r="J34" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K34" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="L34" s="16" t="s">
+      <c r="K34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M34" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="N34" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O34" s="16" t="s">
-        <v>121</v>
+      <c r="M34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N34" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O34" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P34" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q34" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="R34" s="21"/>
-      <c r="S34" s="21"/>
-      <c r="T34" s="21"/>
-      <c r="U34" s="21"/>
-      <c r="V34" s="21"/>
-      <c r="W34" s="21"/>
-      <c r="X34" s="21"/>
-      <c r="Y34" s="21"/>
-      <c r="Z34" s="21"/>
+      <c r="Q34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R34" s="10"/>
+      <c r="S34" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
     </row>
     <row r="35" spans="1:26" ht="14.25" customHeight="1">
       <c r="A35" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>127</v>
+      <c r="B35" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F35" s="12">
-        <v>36.904629999999997</v>
-      </c>
-      <c r="G35" s="12">
-        <v>-75.712649999999996</v>
-      </c>
-      <c r="H35" s="18" t="s">
+      <c r="D35" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="9">
+        <v>38.743299999999998</v>
+      </c>
+      <c r="G35" s="9">
+        <v>-76.707400000000007</v>
+      </c>
+      <c r="H35" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J35" s="16" t="s">
+      <c r="I35" s="8">
+        <v>2003</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K35" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L35" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="M35" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N35" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O35" s="16" t="s">
-        <v>131</v>
+      <c r="M35" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P35" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q35" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="R35" s="29"/>
-      <c r="S35" s="29"/>
-      <c r="T35" s="29"/>
-      <c r="U35" s="29"/>
-      <c r="V35" s="29"/>
-      <c r="W35" s="29"/>
-      <c r="X35" s="29"/>
-      <c r="Y35" s="29"/>
-      <c r="Z35" s="29"/>
+      <c r="Q35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R35" s="10"/>
+      <c r="S35" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
     </row>
     <row r="36" spans="1:26" ht="14.25" customHeight="1">
       <c r="A36" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="28" t="s">
-        <v>133</v>
+      <c r="B36" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F36" s="12">
-        <v>36.945230000000002</v>
-      </c>
-      <c r="G36" s="12">
-        <v>-76.391450000000006</v>
-      </c>
-      <c r="H36" s="18" t="s">
+      <c r="D36" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" s="9">
+        <v>39.228200000000001</v>
+      </c>
+      <c r="G36" s="9">
+        <v>-76.400599999999997</v>
+      </c>
+      <c r="H36" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J36" s="16" t="s">
+      <c r="I36" s="8">
+        <v>2015</v>
+      </c>
+      <c r="J36" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K36" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L36" s="16" t="s">
+      <c r="K36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L36" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M36" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N36" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O36" s="16" t="s">
-        <v>131</v>
+      <c r="M36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N36" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O36" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P36" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q36" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="R36" s="29"/>
-      <c r="S36" s="29"/>
-      <c r="T36" s="29"/>
-      <c r="U36" s="29"/>
-      <c r="V36" s="29"/>
-      <c r="W36" s="29"/>
-      <c r="X36" s="29"/>
-      <c r="Y36" s="29"/>
-      <c r="Z36" s="29"/>
+      <c r="Q36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R36" s="10"/>
+      <c r="S36" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
     </row>
     <row r="37" spans="1:26" ht="14.25" customHeight="1">
       <c r="A37" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="28" t="s">
-        <v>135</v>
+      <c r="B37" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="12">
-        <v>37.787990000000001</v>
-      </c>
-      <c r="G37" s="12">
-        <v>-75.973500000000001</v>
-      </c>
-      <c r="H37" s="18" t="s">
+      <c r="D37" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="9">
+        <v>38.703699999999998</v>
+      </c>
+      <c r="G37" s="9">
+        <v>-76.345299999999995</v>
+      </c>
+      <c r="H37" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I37" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J37" s="16" t="s">
+      <c r="I37" s="8">
+        <v>2017</v>
+      </c>
+      <c r="J37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K37" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L37" s="16" t="s">
+      <c r="K37" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M37" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N37" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O37" s="16" t="s">
-        <v>131</v>
+      <c r="M37" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N37" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O37" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P37" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q37" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="R37" s="29"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="29"/>
-      <c r="Y37" s="29"/>
-      <c r="Z37" s="29"/>
+      <c r="Q37" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R37" s="10"/>
+      <c r="S37" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
     </row>
     <row r="38" spans="1:26" ht="14.25" customHeight="1">
       <c r="A38" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="28" t="s">
-        <v>137</v>
+      <c r="B38" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D38" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F38" s="12">
-        <v>36.9178</v>
-      </c>
-      <c r="G38" s="12">
-        <v>-76.090450000000004</v>
-      </c>
-      <c r="H38" s="18" t="s">
+      <c r="D38" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="9">
+        <v>38.441800000000001</v>
+      </c>
+      <c r="G38" s="9">
+        <v>-76.302899999999994</v>
+      </c>
+      <c r="H38" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I38" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J38" s="16" t="s">
+      <c r="I38" s="8">
+        <v>2017</v>
+      </c>
+      <c r="J38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K38" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L38" s="16" t="s">
+      <c r="K38" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L38" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M38" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N38" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O38" s="16" t="s">
-        <v>131</v>
+      <c r="M38" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N38" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O38" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P38" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q38" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-      <c r="W38" s="29"/>
-      <c r="X38" s="29"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
+      <c r="Q38" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R38" s="10"/>
+      <c r="S38" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
     </row>
     <row r="39" spans="1:26" ht="14.25" customHeight="1">
       <c r="A39" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="28" t="s">
-        <v>139</v>
+      <c r="B39" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F39" s="12">
-        <v>38.326990000000002</v>
-      </c>
-      <c r="G39" s="12">
-        <v>-75.083209999999994</v>
-      </c>
-      <c r="H39" s="18" t="s">
+      <c r="D39" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" s="9">
+        <v>39.353900000000003</v>
+      </c>
+      <c r="G39" s="9">
+        <v>-76.129599999999996</v>
+      </c>
+      <c r="H39" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J39" s="16" t="s">
+      <c r="I39" s="8">
+        <v>2015</v>
+      </c>
+      <c r="J39" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K39" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L39" s="16" t="s">
+      <c r="K39" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L39" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M39" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N39" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O39" s="16" t="s">
-        <v>131</v>
+      <c r="M39" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O39" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P39" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q39" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="R39" s="29"/>
-      <c r="S39" s="29"/>
-      <c r="T39" s="29"/>
-      <c r="U39" s="29"/>
-      <c r="V39" s="29"/>
-      <c r="W39" s="29"/>
-      <c r="X39" s="29"/>
-      <c r="Y39" s="29"/>
-      <c r="Z39" s="29"/>
+      <c r="Q39" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R39" s="10"/>
+      <c r="S39" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
     </row>
     <row r="40" spans="1:26" ht="14.25" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="28" t="s">
-        <v>141</v>
+      <c r="B40" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F40" s="12">
-        <v>36.927059999999997</v>
-      </c>
-      <c r="G40" s="12">
-        <v>-76.006649999999993</v>
-      </c>
-      <c r="H40" s="18" t="s">
+      <c r="D40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="9">
+        <v>39.372300000000003</v>
+      </c>
+      <c r="G40" s="9">
+        <v>-75.8399</v>
+      </c>
+      <c r="H40" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I40" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J40" s="18" t="s">
+      <c r="I40" s="8">
+        <v>2007</v>
+      </c>
+      <c r="J40" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K40" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L40" s="16" t="s">
+      <c r="K40" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L40" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M40" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N40" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O40" s="16" t="s">
-        <v>131</v>
+      <c r="M40" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N40" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O40" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P40" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q40" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="R40" s="29"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="29"/>
-      <c r="U40" s="29"/>
-      <c r="V40" s="29"/>
-      <c r="W40" s="29"/>
-      <c r="X40" s="29"/>
-      <c r="Y40" s="29"/>
-      <c r="Z40" s="29"/>
+      <c r="Q40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R40" s="10"/>
+      <c r="S40" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="11"/>
+      <c r="X40" s="11"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="11"/>
     </row>
     <row r="41" spans="1:26" ht="14.25" customHeight="1">
       <c r="A41" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="28" t="s">
-        <v>143</v>
+      <c r="B41" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F41" s="12">
-        <v>37.601660000000003</v>
-      </c>
-      <c r="G41" s="12">
-        <v>-75.68974</v>
-      </c>
-      <c r="H41" s="18" t="s">
+      <c r="D41" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F41" s="9">
+        <v>38.148299999999999</v>
+      </c>
+      <c r="G41" s="9">
+        <v>-75.286199999999994</v>
+      </c>
+      <c r="H41" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I41" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J41" s="16" t="s">
+      <c r="I41" s="8">
+        <v>2005</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L41" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K41" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L41" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="M41" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N41" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O41" s="16" t="s">
-        <v>131</v>
+      <c r="M41" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P41" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q41" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="R41" s="29"/>
-      <c r="S41" s="29"/>
-      <c r="T41" s="29"/>
-      <c r="U41" s="29"/>
-      <c r="V41" s="29"/>
-      <c r="W41" s="29"/>
-      <c r="X41" s="29"/>
-      <c r="Y41" s="29"/>
-      <c r="Z41" s="29"/>
+      <c r="Q41" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R41" s="10"/>
+      <c r="S41" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+      <c r="W41" s="11"/>
+      <c r="X41" s="11"/>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="11"/>
     </row>
     <row r="42" spans="1:26" ht="14.25" customHeight="1">
       <c r="A42" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B42" s="28" t="s">
-        <v>145</v>
+      <c r="B42" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F42" s="12">
-        <v>36.589709999999997</v>
-      </c>
-      <c r="G42" s="12">
-        <v>-76.020989999999998</v>
-      </c>
-      <c r="H42" s="18" t="s">
+      <c r="D42" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="9">
+        <v>38.267400000000002</v>
+      </c>
+      <c r="G42" s="9">
+        <v>-75.198099999999997</v>
+      </c>
+      <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J42" s="16" t="s">
+      <c r="I42" s="8">
+        <v>2006</v>
+      </c>
+      <c r="J42" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K42" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L42" s="16" t="s">
+      <c r="K42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L42" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M42" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N42" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O42" s="16" t="s">
-        <v>131</v>
+      <c r="M42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N42" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O42" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P42" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q42" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="R42" s="29"/>
-      <c r="S42" s="29"/>
-      <c r="T42" s="29"/>
-      <c r="U42" s="29"/>
-      <c r="V42" s="29"/>
-      <c r="W42" s="29"/>
-      <c r="X42" s="29"/>
-      <c r="Y42" s="29"/>
-      <c r="Z42" s="29"/>
+      <c r="Q42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R42" s="10"/>
+      <c r="S42" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="T42" s="11"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="11"/>
+      <c r="X42" s="11"/>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="11"/>
     </row>
     <row r="43" spans="1:26" ht="14.25" customHeight="1">
       <c r="A43" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="28" t="s">
-        <v>147</v>
+      <c r="B43" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D43" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F43" s="12">
-        <v>37.036520000000003</v>
-      </c>
-      <c r="G43" s="12">
-        <v>-76.076660000000004</v>
-      </c>
-      <c r="H43" s="18" t="s">
+      <c r="D43" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" s="9">
+        <v>38.423999999999999</v>
+      </c>
+      <c r="G43" s="9">
+        <v>-75.188599999999994</v>
+      </c>
+      <c r="H43" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J43" s="16" t="s">
+      <c r="I43" s="8">
+        <v>2003</v>
+      </c>
+      <c r="J43" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K43" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L43" s="16" t="s">
+      <c r="K43" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M43" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N43" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O43" s="16" t="s">
-        <v>131</v>
+      <c r="M43" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N43" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O43" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P43" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q43" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="R43" s="29"/>
-      <c r="S43" s="29"/>
-      <c r="T43" s="29"/>
-      <c r="U43" s="29"/>
-      <c r="V43" s="29"/>
-      <c r="W43" s="29"/>
-      <c r="X43" s="29"/>
-      <c r="Y43" s="29"/>
-      <c r="Z43" s="29"/>
+      <c r="Q43" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R43" s="10"/>
+      <c r="S43" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="11"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="11"/>
     </row>
     <row r="44" spans="1:26" ht="14.25" customHeight="1">
       <c r="A44" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="28" t="s">
-        <v>149</v>
+      <c r="B44" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D44" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F44" s="12">
-        <v>36.830370000000002</v>
-      </c>
-      <c r="G44" s="12">
-        <v>-75.966570000000004</v>
-      </c>
-      <c r="H44" s="18" t="s">
+      <c r="D44" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="9">
+        <v>38.448999999999998</v>
+      </c>
+      <c r="G44" s="9">
+        <v>-75.132499999999993</v>
+      </c>
+      <c r="H44" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I44" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J44" s="16" t="s">
+      <c r="I44" s="8">
+        <v>2008</v>
+      </c>
+      <c r="J44" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K44" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L44" s="16" t="s">
+      <c r="K44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L44" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M44" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N44" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="O44" s="16" t="s">
-        <v>131</v>
+      <c r="M44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N44" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O44" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="P44" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q44" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="R44" s="29"/>
-      <c r="S44" s="29"/>
-      <c r="T44" s="29"/>
-      <c r="U44" s="29"/>
-      <c r="V44" s="29"/>
-      <c r="W44" s="29"/>
-      <c r="X44" s="29"/>
-      <c r="Y44" s="29"/>
-      <c r="Z44" s="29"/>
+      <c r="Q44" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="R44" s="10"/>
+      <c r="S44" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -3183,10 +3887,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{102336CA-9A02-4570-8B99-7823130A0830}">
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="A16" sqref="A6:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3196,6 +3900,7 @@
     <col min="3" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -3509,710 +4214,6 @@
       <c r="X5" s="21"/>
       <c r="Y5" s="21"/>
       <c r="Z5" s="21"/>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="9">
-        <v>38.795999999999999</v>
-      </c>
-      <c r="G6" s="9">
-        <v>-76.720799999999997</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="8">
-        <v>2003</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="10"/>
-      <c r="S6" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="9">
-        <v>38.743299999999998</v>
-      </c>
-      <c r="G7" s="9">
-        <v>-76.707400000000007</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="8">
-        <v>2003</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="10"/>
-      <c r="S7" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="9">
-        <v>39.228200000000001</v>
-      </c>
-      <c r="G8" s="9">
-        <v>-76.400599999999997</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="8">
-        <v>2015</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" s="10"/>
-      <c r="S8" s="36" t="s">
-        <v>169</v>
-      </c>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="9">
-        <v>38.703699999999998</v>
-      </c>
-      <c r="G9" s="9">
-        <v>-76.345299999999995</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="8">
-        <v>2017</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q9" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R9" s="10"/>
-      <c r="S9" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="9">
-        <v>38.441800000000001</v>
-      </c>
-      <c r="G10" s="9">
-        <v>-76.302899999999994</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="8">
-        <v>2017</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R10" s="10"/>
-      <c r="S10" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="9">
-        <v>39.353900000000003</v>
-      </c>
-      <c r="G11" s="9">
-        <v>-76.129599999999996</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="8">
-        <v>2015</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R11" s="10"/>
-      <c r="S11" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="9">
-        <v>39.372300000000003</v>
-      </c>
-      <c r="G12" s="9">
-        <v>-75.8399</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="8">
-        <v>2007</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R12" s="10"/>
-      <c r="S12" s="37" t="s">
-        <v>171</v>
-      </c>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="9">
-        <v>38.148299999999999</v>
-      </c>
-      <c r="G13" s="9">
-        <v>-75.286199999999994</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="8">
-        <v>2005</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R13" s="10"/>
-      <c r="S13" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="9">
-        <v>38.267400000000002</v>
-      </c>
-      <c r="G14" s="9">
-        <v>-75.198099999999997</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="8">
-        <v>2006</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R14" s="10"/>
-      <c r="S14" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="9">
-        <v>38.423999999999999</v>
-      </c>
-      <c r="G15" s="9">
-        <v>-75.188599999999994</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="8">
-        <v>2003</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R15" s="10"/>
-      <c r="S15" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="9">
-        <v>38.448999999999998</v>
-      </c>
-      <c r="G16" s="9">
-        <v>-75.132499999999993</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="8">
-        <v>2008</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P16" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q16" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R16" s="10"/>
-      <c r="S16" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>